<commit_message>
feat: Mercado Livre bot added
</commit_message>
<xml_diff>
--- a/ProjectTemplate/bin/Debug/net8.0/Telegram_Report.xlsx
+++ b/ProjectTemplate/bin/Debug/net8.0/Telegram_Report.xlsx
@@ -34,28 +34,34 @@
     <x:t>SearchText</x:t>
   </x:si>
   <x:si>
+    <x:t>PlayStation DualSense Controle sem fio Edge™</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4,8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Amazon</x:t>
+  </x:si>
+  <x:si>
+    <x:t>29/10/2024</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Plastation 5 slim</x:t>
+  </x:si>
+  <x:si>
     <x:t>Placa de Vídeo Galax NVIDIA GeForce - RTX 3050, 6GB, DDR6, 96 Bits</x:t>
   </x:si>
   <x:si>
-    <x:t>4,8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Amazon</x:t>
-  </x:si>
-  <x:si>
-    <x:t>24/10/2024</x:t>
-  </x:si>
-  <x:si>
     <x:t>Placa de Vídeo RTX 3060</x:t>
   </x:si>
   <x:si>
-    <x:t>Processador AMD Ryzen 5 5600G, 3.9GHz (4.4GHz Max Turbo), AM4, Vídeo Integrado</x:t>
+    <x:t>ProcessadorAMD Ryzen 7 5700X, 8 núcleos 16 threads, arquitetura Zen 3, processador de alto desempenho com suporte cache de 36 MB</x:t>
   </x:si>
   <x:si>
     <x:t>Processador Ryzen 5 7600 AM5</x:t>
   </x:si>
   <x:si>
-    <x:t>Placa Mãe Gigabyte B760M AORUS ELITE (rev. 1.0), LGA 1700, DDR5</x:t>
+    <x:t>Placa Mãe Asus TUF GAMING B650M-E (AM5/4xDDR5/HDMI/DP/M.2/USB 3.2)</x:t>
   </x:si>
   <x:si>
     <x:t>4,4</x:t>
@@ -106,7 +112,7 @@
     <x:t>SSD sata 1TB</x:t>
   </x:si>
   <x:si>
-    <x:t>GIGABYTE Placa gráfica Radeon RX 6500 XT Eagle 4G, sistema de resfriamento WINDFORCE 2X, placa de vídeo GDDR6 de 64 bits de 4 GB, GV-R65XTEAGLE-4GD</x:t>
+    <x:t>PLACA DE VÍDEO SAPPHIRE PULSE AMD RADEON RX 6400 GRAPHICS CARD GDDR6 1080 FHD 4GB PCIE 4.0 HDMI</x:t>
   </x:si>
   <x:si>
     <x:t>4,2</x:t>
@@ -115,76 +121,118 @@
     <x:t>Placa de vídeo AMD radeon RX 7900</x:t>
   </x:si>
   <x:si>
+    <x:t>Console Playstation 5 Sony Slim, SSD 1TB, Controle Sem Fio Dualsense, Edição Digital, Branco, Returnal E Ratchet E Clank</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kabum</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Placa de Vídeo MSI RTX 3050 Ventus 2X XS OC NVIDIA GeForce, 8GB GDDR6 - 912-V809-4266</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Processador AMD Ryzen 5 5600, 3.5GHz (4.4GHz Turbo), AM4 - 100-100000927BOX</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Placa Mãe Asrock B550m Pg Riptide, AMD AM4, MATX, DDR4, Chipset B550</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Placa de Vídeo Palit Geforce GTX 1050 TI Stormx, 4GB, GDDR5, 128 Bits - NE5105T018G1-1070F</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kit PC Completo com Processador AMD Ryzen 3 3200g, Placa Mãe A520M-A PRO AM4, 4GB DDR4, SSD 120GB, Fonte 500W, Gabinete Gamer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Memória RAM 8GB KBM! Gaming, Preto, 3200 MHz, DDR4, CL22 - KGRM32000822PT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Memória RAM 16GB KBM! Gaming, Preto, 3200 MHz, DDR4, CL22 - KGRM32001622PT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SSD 1TB Kingston Nv2, M.2 2280 PCIe, NVMe, Leitura 3500MB/s, Gravação 2100MB/s - Snv2s/1000g</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SSD SATA Crucial BX500, 1TB, 2.5", Leitura: 540MB/s e Gravação: 500MB/s, Preto - CT1000BX500SSD1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Placa de Vídeo RX 7900XTX BLACK Gaming 24G XFX Speedster MERC310 AMD Radeon, 24GB DDR6, 3 FAN - RX-79XMERCB9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sony PlayStation 3 Slim 160GB Standard cor charcoal black 2010</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4.9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mercado Livre</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Placa De Video Gpu Nvidia Geforce Rtx 3050 6gb Gddr6 96bits</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Processador gamer AMD Ryzen 5 7600 100-100001015BOX de 6 núcleos e 5.1GHz de frequência com gráfica integrada</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5.0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Placa-mãe Asrock B650m H M.2 + Am5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3.7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Placa De Vídeo Nvidia Galax Geforce 10 Series Gtx 1060 60nr</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Processador gamer AMD Ryzen 3 3200G YD3200C5FHBOX de 4 núcleos e 4GHz de frequência com gráfica integrada</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4.8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Memória RAM Kingston 8GB Ddr3 1600mhz Pc3 12800 KVR16N11/8 PC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Memória RAM 16GB Dell 2RX8 DDR4 2666MHZ UDIMM SNPVDFYDC/16G</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SSD Nvme Asgard AN4 1tb Gen4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Disco sólido interno SanDisk SSD Plus SDSSDA-1T00-G27 1TB preto</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Placa De Vídeo Rx 570 Pcyes Amd Radeon 4gb Gddr5 128bits</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Console Sony PlayStation 5 Slim, Branco + 2 Jogos - 1000038899</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Magazine Luiza</x:t>
+  </x:si>
+  <x:si>
     <x:t>Placa de Vídeo RTX 3060 1-Click OC Galax NVIDIA GeForce, 12GB GDDR6, LHR, DLSS, Ray Tracing - 36NOL7MD1VOC</x:t>
   </x:si>
   <x:si>
-    <x:t>5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kabum</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Processador AMD Ryzen 5 5600, 3.5GHz (4.4GHz Turbo), AM4 - 100-100000927BOX</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Placa-Mãe AsRock B550M Steel Legend, AMD AM4 B550, DDR4 4733 OC, USB 3.2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Placa de Vídeo Gainward NVIDIA GeForce GTX 1050 TI, 4GB GDDR5, 128 Bits - NE5105T018G1-1070F</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kit PC Completo com Processador AMD Ryzen 3 3200g, Placa Mãe A520M-A PRO AM4, 4GB DDR4, SSD 120GB, Fonte 500W, Gabinete Gamer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Memória RAM 8GB KBM! Gaming, Preto, 3200 MHz, DDR4, CL22 - KGRM32000822PT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Memória RAM 16GB KBM! Gaming, Preto, 3200 MHz, DDR4, CL22 - KGRM32001622PT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SSD Kingston KC3000, 1 TB, M.2 2280, PCIe 4.0 x4, NVMe, Leitura: 7000 MB/s, Gravação: 6000 MB/s, Preto - SKC3000S/1024G</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SSD SATA Crucial BX500, 1TB, 2.5", Leitura: 540MB/s e Gravação: 500MB/s, Preto - CT1000BX500SSD1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Placa de Vídeo RX 7900XTX BLACK Gaming 24G XFX Speedster MERC310 AMD Radeon, 24GB DDR6, 3 FAN - RX-79XMERCB9</x:t>
+    <x:t>Processador AMD Ryzen 5 7600 AM5 6C/12T</x:t>
   </x:si>
   <x:si>
     <x:t>n/a</x:t>
   </x:si>
   <x:si>
-    <x:t>Magazine Luiza</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Processador AMD Ryzen 5 7600 AM5 6C/12T</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4.5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Processador AMD Ryzen 3 3200G 3.6GHz (4GHz Max Turbo) 6MB Socket AM4 - YD3200C5FHBOX</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Memória RAM Rise Mode Z, 8GB, 3200MHz, DDR4, CL19, Preto - RM-D4-8G-3200Z</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4.4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Memória Corsair Vengeance 16GB, 2400MHz, DDR4, C16, para Notebook, Preto - CMSX16GX4M1A2400C16</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5.0</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SSD NVMe M.2 PUSKILL - Alta Velocidade - 1TB, 512GB, 256GB e 128GB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ssd 1tb 2.5" sata iii ns100 lexar</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Placa de Video ASROCK Radeon RX 7900XT Phantom Gaming 20GB OC GDDR6 320 BITS - 90-GA3XZZ-00UANF</x:t>
+    <x:t>4.6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Processador AMD Ryzen 3 3200G 3.60GHz - 4.00GHz Turbo 4MB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Memória RAM 8GB 1 para desktops e cpus NET48192UD24</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hd Ssd 1TB SATA III Goldenfir Desktop Notebook</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -566,7 +614,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B2" s="0">
-        <x:v>1285</x:v>
+        <x:v>1127</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
         <x:v>7</x:v>
@@ -586,7 +634,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="B3" s="0">
-        <x:v>1099</x:v>
+        <x:v>1285</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
         <x:v>7</x:v>
@@ -606,10 +654,10 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="B4" s="0">
-        <x:v>1109</x:v>
+        <x:v>1029</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
         <x:v>8</x:v>
@@ -618,18 +666,18 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="F4" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:6">
       <x:c r="A5" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B5" s="0">
+        <x:v>1099</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
         <x:v>16</x:v>
-      </x:c>
-      <x:c r="B5" s="0">
-        <x:v>1000</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>17</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
         <x:v>8</x:v>
@@ -638,18 +686,18 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="F5" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:6">
       <x:c r="A6" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B6" s="0">
+        <x:v>1000</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
         <x:v>19</x:v>
-      </x:c>
-      <x:c r="B6" s="0">
-        <x:v>533</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="s">
-        <x:v>17</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
         <x:v>8</x:v>
@@ -666,10 +714,10 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="B7" s="0">
-        <x:v>175</x:v>
+        <x:v>533</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
         <x:v>8</x:v>
@@ -678,18 +726,18 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="F7" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:6">
       <x:c r="A8" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B8" s="0">
+        <x:v>175</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
         <x:v>24</x:v>
-      </x:c>
-      <x:c r="B8" s="0">
-        <x:v>282</x:v>
-      </x:c>
-      <x:c r="C8" s="0" t="s">
-        <x:v>7</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
         <x:v>8</x:v>
@@ -706,7 +754,7 @@
         <x:v>26</x:v>
       </x:c>
       <x:c r="B9" s="0">
-        <x:v>403</x:v>
+        <x:v>282</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
         <x:v>7</x:v>
@@ -726,7 +774,7 @@
         <x:v>28</x:v>
       </x:c>
       <x:c r="B10" s="0">
-        <x:v>369</x:v>
+        <x:v>414</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
         <x:v>7</x:v>
@@ -746,10 +794,10 @@
         <x:v>30</x:v>
       </x:c>
       <x:c r="B11" s="0">
-        <x:v>1302</x:v>
+        <x:v>369</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
         <x:v>8</x:v>
@@ -758,227 +806,227 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="F11" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:6">
       <x:c r="A12" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B12" s="0">
+        <x:v>1245</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="B12" s="0">
-        <x:v>1639.99</x:v>
-      </x:c>
-      <x:c r="C12" s="0" t="s">
+      <x:c r="D12" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F12" s="0" t="s">
         <x:v>34</x:v>
-      </x:c>
-      <x:c r="D12" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="E12" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="F12" s="0" t="s">
-        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:6">
       <x:c r="A13" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B13" s="0">
+        <x:v>3889</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
         <x:v>36</x:v>
       </x:c>
-      <x:c r="B13" s="0">
-        <x:v>908.76</x:v>
-      </x:c>
-      <x:c r="C13" s="0" t="s">
-        <x:v>34</x:v>
-      </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="E13" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="F13" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:6">
       <x:c r="A14" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B14" s="0">
+        <x:v>1299.99</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="B14" s="0">
-        <x:v>1612.53</x:v>
-      </x:c>
-      <x:c r="C14" s="0" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="D14" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
       <x:c r="E14" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="F14" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:6">
       <x:c r="A15" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="B15" s="0">
-        <x:v>1068.93</x:v>
+        <x:v>908.76</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="E15" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="F15" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:6">
       <x:c r="A16" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="B16" s="0">
-        <x:v>1498.99</x:v>
+        <x:v>988.5</x:v>
       </x:c>
       <x:c r="C16" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="E16" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="F16" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:6">
       <x:c r="A17" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="B17" s="0">
-        <x:v>124.99</x:v>
+        <x:v>1462.12</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="E17" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="F17" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:6">
       <x:c r="A18" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="B18" s="0">
-        <x:v>249.99</x:v>
+        <x:v>1399.98</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="E18" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="F18" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:6">
       <x:c r="A19" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="B19" s="0">
-        <x:v>689.99</x:v>
+        <x:v>124.99</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="E19" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="F19" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:6">
       <x:c r="A20" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="B20" s="0">
-        <x:v>479.99</x:v>
+        <x:v>249.99</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="E20" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="F20" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:6">
       <x:c r="A21" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="B21" s="0">
-        <x:v>6999.99</x:v>
+        <x:v>422.96</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="E21" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="F21" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:6">
       <x:c r="A22" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="B22" s="0">
-        <x:v>0</x:v>
+        <x:v>479.99</x:v>
       </x:c>
       <x:c r="C22" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="D22" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="E22" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="F22" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:6">
@@ -986,179 +1034,459 @@
         <x:v>47</x:v>
       </x:c>
       <x:c r="B23" s="0">
-        <x:v>2275.9</x:v>
+        <x:v>6999.99</x:v>
       </x:c>
       <x:c r="C23" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="E23" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="F23" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:6">
       <x:c r="A24" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="B24" s="0">
-        <x:v>0</x:v>
+        <x:v>1128</x:v>
       </x:c>
       <x:c r="C24" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="D24" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="E24" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="F24" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:6">
       <x:c r="A25" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="B25" s="0">
-        <x:v>0</x:v>
+        <x:v>1729</x:v>
       </x:c>
       <x:c r="C25" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="D25" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="E25" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="F25" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:6">
       <x:c r="A26" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="B26" s="0">
-        <x:v>678.99</x:v>
+        <x:v>1499</x:v>
       </x:c>
       <x:c r="C26" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="D26" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="E26" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="F26" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:6">
       <x:c r="A27" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B27" s="0">
+        <x:v>1005</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="s">
         <x:v>50</x:v>
       </x:c>
-      <x:c r="B27" s="0">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="C27" s="0" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="D27" s="0" t="s">
-        <x:v>46</x:v>
-      </x:c>
       <x:c r="E27" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="F27" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:6">
       <x:c r="A28" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="B28" s="0">
-        <x:v>289.99</x:v>
+        <x:v>1057</x:v>
       </x:c>
       <x:c r="C28" s="0" t="s">
         <x:v>53</x:v>
       </x:c>
       <x:c r="D28" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="E28" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="F28" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:6">
       <x:c r="A29" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="B29" s="0">
-        <x:v>143.17</x:v>
+        <x:v>491</x:v>
       </x:c>
       <x:c r="C29" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="D29" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="E29" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="F29" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:6">
       <x:c r="A30" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="B30" s="0">
-        <x:v>640.29</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="C30" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="D30" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="E30" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="F30" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:6">
       <x:c r="A31" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="B31" s="0">
-        <x:v>9258.51</x:v>
+        <x:v>1088</x:v>
       </x:c>
       <x:c r="C31" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="D31" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="E31" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="F31" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>27</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:6">
+      <x:c r="A32" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="B32" s="0">
+        <x:v>598</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="D32" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="E32" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F32" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:6">
+      <x:c r="A33" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="B33" s="0">
+        <x:v>575</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="E33" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F33" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:6">
+      <x:c r="A34" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B34" s="0">
+        <x:v>1039</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="D34" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="E34" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F34" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:6">
+      <x:c r="A35" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="B35" s="0">
+        <x:v>3876.47</x:v>
+      </x:c>
+      <x:c r="C35" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="D35" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="E35" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F35" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:6">
+      <x:c r="A36" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="B36" s="0">
+        <x:v>1639.99</x:v>
+      </x:c>
+      <x:c r="C36" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="D36" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="E36" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F36" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:6">
+      <x:c r="A37" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="B37" s="0">
+        <x:v>2275.9</x:v>
+      </x:c>
+      <x:c r="C37" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="D37" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="E37" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F37" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:6">
+      <x:c r="A38" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="B38" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="C38" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="D38" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="E38" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F38" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:6">
+      <x:c r="A39" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="B39" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="C39" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="D39" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="E39" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F39" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:6">
+      <x:c r="A40" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="B40" s="0">
+        <x:v>699.99</x:v>
+      </x:c>
+      <x:c r="C40" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="D40" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="E40" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F40" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:6">
+      <x:c r="A41" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="B41" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="C41" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="D41" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="E41" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F41" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:6">
+      <x:c r="A42" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="B42" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="C42" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="D42" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="E42" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F42" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:6">
+      <x:c r="A43" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="B43" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="C43" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="D43" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="E43" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F43" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:6">
+      <x:c r="A44" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="B44" s="0">
+        <x:v>399.9</x:v>
+      </x:c>
+      <x:c r="C44" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="D44" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="E44" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F44" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:6">
+      <x:c r="A45" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="B45" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="C45" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="D45" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="E45" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F45" s="0" t="s">
+        <x:v>34</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>